<commit_message>
Tableau de Synthese + Rapport de stage Turgot (modifier)
</commit_message>
<xml_diff>
--- a/assets/TableauSyntheseE4.xlsx
+++ b/assets/TableauSyntheseE4.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -116,19 +116,22 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">AWS EC2 site dymamique Perso</t>
+    <t xml:space="preserve">Veille Techno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coder un nouveau besion (MMA)</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">Coder un nouveau besion (TP Resto)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
-    <t xml:space="preserve">Modelisation (modelio)</t>
+    <t xml:space="preserve">Processus de modélisation BPMN (modelio)</t>
   </si>
   <si>
     <t xml:space="preserve">Créer un site web de A à Z</t>
@@ -140,13 +143,10 @@
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t xml:space="preserve">mise emplace du projet avec Githud</t>
+    <t xml:space="preserve">mise enplace du projet avec Github</t>
   </si>
   <si>
     <t xml:space="preserve">Auto formation avec Angular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X </t>
   </si>
 </sst>
 </file>
@@ -245,6 +245,12 @@
       <sz val="26"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -266,12 +272,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="26"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -595,7 +595,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -692,6 +692,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -700,36 +708,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1015,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,24 +1172,28 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="23"/>
+      <c r="H9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="24"/>
     </row>
     <row r="10" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="20"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="24"/>
+      <c r="G10" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="19"/>
@@ -1195,7 +1203,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
@@ -1205,7 +1213,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="19"/>
@@ -1215,7 +1223,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19"/>
@@ -1225,7 +1233,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
@@ -1235,7 +1243,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="19"/>
@@ -1245,7 +1253,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
@@ -1255,7 +1263,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
@@ -1265,51 +1273,51 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" s="17" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="A19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="27" t="n">
+      <c r="A20" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="29" t="n">
         <v>45426</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="29" t="s">
-        <v>25</v>
+      <c r="F20" s="31" t="s">
+        <v>27</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="32" t="s">
         <v>30</v>
       </c>
+      <c r="B21" s="33" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="22"/>
-      <c r="D21" s="32" t="s">
-        <v>25</v>
+      <c r="D21" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
@@ -1319,7 +1327,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="19"/>
@@ -1329,7 +1337,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
@@ -1339,7 +1347,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
@@ -1349,7 +1357,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
@@ -1359,37 +1367,39 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" s="17" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
+      <c r="A27" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="20"/>
-      <c r="C28" s="33" t="s">
-        <v>25</v>
+      <c r="C28" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+      <c r="F28" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="G28" s="22"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
@@ -1397,8 +1407,8 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="34" t="s">
-        <v>34</v>
+      <c r="H29" s="35" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1409,7 +1419,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19"/>
@@ -1419,7 +1429,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="19"/>
@@ -1429,7 +1439,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
@@ -1439,27 +1449,27 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="35"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
     </row>
     <row r="35" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
     </row>
     <row r="36" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
changement des nom des epreve E4 et E5 + nouveau tableau de Syntese
</commit_message>
<xml_diff>
--- a/assets/TableauSyntheseE4.xlsx
+++ b/assets/TableauSyntheseE4.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">X SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse URL du portfolio :</t>
+    <t xml:space="preserve">Adresse URL du portfolio : hammami-rayan.github.io/portfolio</t>
   </si>
   <si>
     <t xml:space="preserve">Compétences mises en œuvre
@@ -128,6 +128,9 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
+    <t xml:space="preserve">AWS cloud fondation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
@@ -147,6 +150,12 @@
   </si>
   <si>
     <t xml:space="preserve">Auto formation avec Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet GSB suivi de frais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">déploiement du protfolio sur GitPage</t>
   </si>
 </sst>
 </file>
@@ -595,7 +604,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -689,55 +698,51 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1019,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1182,28 +1187,30 @@
         <v>26</v>
       </c>
       <c r="B10" s="20"/>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="25" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="22"/>
-      <c r="G10" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="G10" s="23"/>
       <c r="H10" s="26"/>
     </row>
     <row r="11" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
+      <c r="A11" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="B11" s="20"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="26"/>
+      <c r="H11" s="27" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="19"/>
@@ -1276,45 +1283,47 @@
       <c r="H18" s="26"/>
     </row>
     <row r="19" s="17" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="A19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="29" t="n">
+      <c r="A20" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="30" t="n">
         <v>45426</v>
       </c>
-      <c r="C20" s="30"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="32" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="26"/>
     </row>
     <row r="21" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="33" t="s">
         <v>31</v>
       </c>
+      <c r="B21" s="34" t="s">
+        <v>32</v>
+      </c>
       <c r="C21" s="22"/>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="22"/>
+      <c r="E21" s="32" t="s">
+        <v>27</v>
+      </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="26"/>
@@ -1370,28 +1379,30 @@
       <c r="H26" s="26"/>
     </row>
     <row r="27" s="17" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+      <c r="A27" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="20"/>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="32" t="s">
+        <v>27</v>
+      </c>
       <c r="E28" s="22"/>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="23" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="22"/>
@@ -1399,7 +1410,7 @@
     </row>
     <row r="29" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
@@ -1407,28 +1418,38 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19"/>
+      <c r="A30" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+      <c r="D30" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>27</v>
+      </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="26"/>
     </row>
     <row r="31" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19"/>
+      <c r="A31" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="G31" s="32" t="s">
+        <v>27</v>
+      </c>
       <c r="H31" s="26"/>
     </row>
     <row r="32" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1452,24 +1473,24 @@
       <c r="H33" s="26"/>
     </row>
     <row r="34" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
     </row>
     <row r="35" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
     </row>
     <row r="36" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>